<commit_message>
change grid to 5*4
</commit_message>
<xml_diff>
--- a/Cricket-Auction-App/auction_results.xlsx
+++ b/Cricket-Auction-App/auction_results.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,14 +468,14 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="B2" t="n">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rittik Rahaman </t>
+          <t xml:space="preserve">Rahul Chattaraj </t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -484,24 +484,24 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>500</v>
+        <v>20</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-09-02 23:10:48</t>
+          <t>2025-09-02 23:37:51</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B3" t="n">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Chandan yadav </t>
+          <t xml:space="preserve">Abhradip Maji </t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -510,24 +510,24 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>400</v>
+        <v>20</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-09-02 23:11:07</t>
+          <t>2025-09-02 23:38:30</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B4" t="n">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Koushik Saha</t>
+          <t xml:space="preserve">Debojyoti Saha </t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -536,24 +536,24 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>1000</v>
+        <v>20</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-09-02 23:16:52</t>
+          <t>2025-09-02 23:38:38</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B5" t="n">
-        <v>58</v>
+        <v>112</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dibakar Roy </t>
+          <t xml:space="preserve">SAGEN MURMU </t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -562,11 +562,349 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-09-02 23:17:12</t>
+          <t>2025-09-02 23:38:51</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>115</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anupam Ghosh </t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>madhu</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>20</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-09-02 23:39:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>116</v>
+      </c>
+      <c r="B7" t="n">
+        <v>82</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Biplab Senapati </t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>madhu</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>20</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2025-09-02 23:39:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>117</v>
+      </c>
+      <c r="B8" t="n">
+        <v>41</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Ambuj Mahato</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>madhu</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>20</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2025-09-02 23:39:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>118</v>
+      </c>
+      <c r="B9" t="n">
+        <v>94</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>ARKA DEY</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>madhu</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>20</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2025-09-02 23:39:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>119</v>
+      </c>
+      <c r="B10" t="n">
+        <v>83</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>MRIGANKA MAHATO</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>madhu</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>20</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2025-09-02 23:39:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>120</v>
+      </c>
+      <c r="B11" t="n">
+        <v>75</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Amit Das </t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>madhu</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>20</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2025-09-02 23:39:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>121</v>
+      </c>
+      <c r="B12" t="n">
+        <v>51</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AMIT MUKHERJEE </t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>madhu</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>20</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2025-09-02 23:40:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>122</v>
+      </c>
+      <c r="B13" t="n">
+        <v>32</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Rahul Mahato</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>madhu</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>20</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2025-09-02 23:40:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>123</v>
+      </c>
+      <c r="B14" t="n">
+        <v>104</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Suman Mahato </t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>madhu</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>20</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2025-09-02 23:40:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>124</v>
+      </c>
+      <c r="B15" t="n">
+        <v>99</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Asit Kumar Mahato </t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>madhu</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>20</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2025-09-02 23:40:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>125</v>
+      </c>
+      <c r="B16" t="n">
+        <v>33</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anjan Kumar mandal </t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>madhu</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>20</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2025-09-02 23:47:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>126</v>
+      </c>
+      <c r="B17" t="n">
+        <v>37</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nadim Rijbi </t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>madhu</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>20</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2025-09-02 23:47:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>127</v>
+      </c>
+      <c r="B18" t="n">
+        <v>111</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Abhay Mandal </t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>madhu</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>20</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2025-09-02 23:47:51</t>
         </is>
       </c>
     </row>
@@ -581,7 +919,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -608,54 +946,223 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rittik Rahaman </t>
+          <t xml:space="preserve">Rahul Chattaraj </t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>500</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Chandan yadav </t>
+          <t xml:space="preserve">Abhradip Maji </t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>400</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Koushik Saha</t>
+          <t xml:space="preserve">Debojyoti Saha </t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1000</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>58</v>
+        <v>112</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dibakar Roy </t>
+          <t xml:space="preserve">SAGEN MURMU </t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>200</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anupam Ghosh </t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>82</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Biplab Senapati </t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>41</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Ambuj Mahato</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>94</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>ARKA DEY</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>83</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>MRIGANKA MAHATO</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>75</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Amit Das </t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>51</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AMIT MUKHERJEE </t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>32</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Rahul Mahato</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>104</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Suman Mahato </t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>99</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Asit Kumar Mahato </t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>33</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anjan Kumar mandal </t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>37</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nadim Rijbi </t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>111</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Abhay Mandal </t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>